<commit_message>
feat. Excel Checkliste minimal angepasst
</commit_message>
<xml_diff>
--- a/Excel/05_03_checkliste.xlsx
+++ b/Excel/05_03_checkliste.xlsx
@@ -8,48 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5AD981-10CF-5E48-A7CF-BD2644D3F20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6140E5-1781-8848-88A2-510FFF6FB359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{824E35B1-06FB-A441-A126-FF76D37EF72C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{824E35B1-06FB-A441-A126-FF76D37EF72C}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
     <sheet name="Raster" sheetId="2" r:id="rId2"/>
     <sheet name="Ergebnis" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Ergebnis!$A$13</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Ergebnis!$A$17:$A$18</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Ergebnis!$D$17:$D$18</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Ergebnis!$E$17:$E$18</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Ergebnis!$A$12:$A$13</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Ergebnis!$A$17:$A$18</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Ergebnis!$B$12:$B$13</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Ergebnis!$B$17:$B$18</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Ergebnis!$D$17:$D$18</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Ergebnis!$E$17:$E$18</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Ergebnis!$A$12:$A$13</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Ergebnis!$A$17:$A$18</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Ergebnis!$B$13</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Ergebnis!$B$12:$B$13</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Ergebnis!$B$17:$B$18</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Ergebnis!$D$17:$D$18</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Ergebnis!$E$17:$E$18</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Ergebnis!$A$17:$A$18</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Ergebnis!$B$12</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Ergebnis!$B$13</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Ergebnis!$B$17:$B$18</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Ergebnis!$D$17:$D$18</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Ergebnis!$E$17:$E$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Ergebnis!$B$17:$B$18</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Ergebnis!$D$17:$D$18</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Ergebnis!$E$17:$E$18</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Ergebnis!$A$12:$A$13</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Ergebnis!$A$17:$A$18</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Ergebnis!$B$12:$B$13</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Ergebnis!$B$17:$B$18</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -298,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -307,7 +275,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,19 +288,19 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -558,7 +525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B1F7028-271B-344A-BA84-D167E85D0EB5}" type="CELLRANGE">
+                    <a:fld id="{C3DB3B5D-64EC-8242-AAEC-CF722118B0E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -577,7 +544,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1621,16 +1587,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>31552</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742752</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>50556</xdr:rowOff>
+      <xdr:rowOff>162316</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>91439</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>182879</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91439</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2192,11 +2158,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}" name="tblMap" displayName="tblMap" ref="A1:B4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}" name="tblMap" displayName="tblMap" ref="A1:B4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:B4" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2E415323-F0F4-DF42-8618-DFC330E24A9F}" name="Label" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{2AD24CC9-CE9F-3C47-8031-91B2311661C6}" name="Zahl" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{2E415323-F0F4-DF42-8618-DFC330E24A9F}" name="Label" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2AD24CC9-CE9F-3C47-8031-91B2311661C6}" name="Zahl" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2206,12 +2172,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D91CD661-3334-0F41-A7F6-D541C684E11A}" name="tblRaster" displayName="tblRaster" ref="A1:F10" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:F10" xr:uid="{D91CD661-3334-0F41-A7F6-D541C684E11A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{48EC3C85-0478-E24F-8C6C-9E9150301F82}" name="Zusatzdimension" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{2B1F30E9-8D65-194C-8994-DEC140EDE5E1}" name="Unterdimension" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{B5FF6543-2649-CE49-AD49-22965AEE247E}" name="Achse" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{48EC3C85-0478-E24F-8C6C-9E9150301F82}" name="Zusatzdimension" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2B1F30E9-8D65-194C-8994-DEC140EDE5E1}" name="Unterdimension" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B5FF6543-2649-CE49-AD49-22965AEE247E}" name="Achse" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{DDD13B20-7639-A54A-84A9-A92CB62DB822}" name="Leitfrage"/>
     <tableColumn id="5" xr3:uid="{A5671AFB-0AFF-BA43-85A5-F8CAA3830C0A}" name="Bewertung"/>
-    <tableColumn id="6" xr3:uid="{9E073365-4767-7540-B07B-6DC0088374EA}" name="Wert" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{9E073365-4767-7540-B07B-6DC0088374EA}" name="Wert" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2596,7 +2562,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="168" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2629,13 +2595,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -2650,13 +2616,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -2671,13 +2637,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2686,19 +2652,19 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -2707,19 +2673,19 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2728,19 +2694,19 @@
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2749,19 +2715,19 @@
       <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2770,19 +2736,19 @@
       <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2791,19 +2757,19 @@
       <c r="E9" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -2812,7 +2778,7 @@
       <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
         <v>3</v>
       </c>
@@ -2858,7 +2824,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2871,18 +2837,18 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="4">
         <v>2.34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="5"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" cm="1">
+      <c r="B3" s="4" cm="1">
         <f t="array" ref="B3">AVERAGE(
   _xlfn._xlws.FILTER(tblRaster[Wert],
     (tblRaster[Achse]="X")+(tblRaster[Achse]="X+Y")
@@ -2895,7 +2861,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" cm="1">
+      <c r="B4" s="4" cm="1">
         <f t="array" ref="B4">AVERAGE(
   _xlfn._xlws.FILTER(tblRaster[Wert],
     (tblRaster[Achse]="Y")+(tblRaster[Achse]="X+Y")
@@ -2905,13 +2871,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="str">
+      <c r="B6" s="4" t="str">
         <f>IF(B3&gt;=$B$1,"hoch","niedrig")</f>
         <v>niedrig</v>
       </c>
@@ -2920,7 +2886,7 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5" t="str">
+      <c r="B7" s="4" t="str">
         <f>IF(B4&gt;=$B$1,"hoch","niedrig")</f>
         <v>niedrig</v>
       </c>
@@ -2929,19 +2895,19 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="str">
+      <c r="B8" s="4" t="str">
         <f>B7&amp;"/"&amp;B6</f>
         <v>niedrig/niedrig</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5" t="str">
+      <c r="B10" s="4" t="str">
         <f>IF(COUNTBLANK(tblRaster[Bewertung])=0,"ok","fehlt")</f>
         <v>ok</v>
       </c>
@@ -3010,7 +2976,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Excel Checkliste Gewichtung eingefügt
</commit_message>
<xml_diff>
--- a/Excel/05_03_checkliste.xlsx
+++ b/Excel/05_03_checkliste.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6140E5-1781-8848-88A2-510FFF6FB359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D2C707-AFB8-544E-82B1-148027F876A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{824E35B1-06FB-A441-A126-FF76D37EF72C}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{824E35B1-06FB-A441-A126-FF76D37EF72C}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
     <sheet name="Raster" sheetId="2" r:id="rId2"/>
     <sheet name="Ergebnis" sheetId="3" r:id="rId3"/>
+    <sheet name="Mapping (2)" sheetId="4" r:id="rId4"/>
+    <sheet name="Raster (2)" sheetId="5" r:id="rId5"/>
+    <sheet name="Ergebnis (2)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
   <si>
     <t>Label</t>
   </si>
@@ -203,7 +206,15 @@
     <t>Y_h</t>
   </si>
   <si>
-    <t>Use Case 1</t>
+    <t>intelligente 
+Build-
+Fehlerdiagnose</t>
+  </si>
+  <si>
+    <t>Gewicht</t>
+  </si>
+  <si>
+    <t>GewichteterWert</t>
   </si>
 </sst>
 </file>
@@ -281,12 +292,126 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -400,6 +525,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00B1A0"/>
       <color rgb="FF009A94"/>
     </mruColors>
   </colors>
@@ -525,7 +651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3DB3B5D-64EC-8242-AAEC-CF722118B0E3}" type="CELLRANGE">
+                    <a:fld id="{C2B70561-BC8A-4043-9D43-A62D9066C001}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -565,7 +691,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="bg1"/>
                     </a:solidFill>
@@ -599,7 +725,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.8571428571428572</c:v>
+                  <c:v>1.5714285714285714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,7 +750,9 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>Use Case 1</c:v>
+                    <c:v>intelligente 
+Build-
+Fehlerdiagnose</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1027,6 +1155,621 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Bewertungsraster</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Use Case</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="58"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B1A0"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat">
+                <a:solidFill>
+                  <a:srgbClr val="009A94"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{9489993D-EBE9-074B-AE6A-4197D1C95890}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-45A0-D44B-869E-5CFACCC037BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ergebnis (2)'!$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ergebnis (2)'!$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'Ergebnis (2)'!$A$26</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>intelligente 
+Build-
+Fehlerdiagnose</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-45A0-D44B-869E-5CFACCC037BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trennlinie X</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ergebnis (2)'!$A$17:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ergebnis (2)'!$B$17:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-45A0-D44B-869E-5CFACCC037BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Trennlinie Y</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ergebnis (2)'!$D$17:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ergebnis (2)'!$E$17:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-45A0-D44B-869E-5CFACCC037BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1490819648"/>
+        <c:axId val="1481579968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1490819648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1100">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Implementierungsaufwand</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.33748594012979705"/>
+              <c:y val="0.9201398706326791"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1481579968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1481579968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1100">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Operativer Mehrwert</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.1374914697670754E-2"/>
+              <c:y val="0.28012711580171279"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1490819648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1067,7 +1810,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2157,28 +3456,636 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742752</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>162316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>91439</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB5CF43A-8311-CD4A-ADE2-CB99857CCFC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16592</cdr:x>
+      <cdr:y>0.25484</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.45867</cdr:x>
+      <cdr:y>0.41563</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Textfeld 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34AA8F33-163E-E8EC-47E1-8CCC21DB05DE}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="755540" y="687641"/>
+          <a:ext cx="1333077" cy="433865"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Hoher Merhwert,</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>geringer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> Aufwand</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1200" kern="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.58972</cdr:x>
+      <cdr:y>0.25484</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.88247</cdr:x>
+      <cdr:y>0.41563</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Textfeld 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D708C1F-3C6A-8387-E132-81315BDB973A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2685378" y="687641"/>
+          <a:ext cx="1333076" cy="433865"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Hoher Merhwert,</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>hoher</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> Aufwand</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1200" kern="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16592</cdr:x>
+      <cdr:y>0.59203</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.45867</cdr:x>
+      <cdr:y>0.75282</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Textfeld 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A65C8D-0CC9-5837-2DFA-111319A2FF83}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="755540" y="1597506"/>
+          <a:ext cx="1333077" cy="433865"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Geringer Merhwert,</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>geringer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> Aufwand</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1200" kern="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.58972</cdr:x>
+      <cdr:y>0.59203</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.88247</cdr:x>
+      <cdr:y>0.75282</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="Textfeld 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C90772C2-58AD-C737-25BE-BAC41C356725}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2685378" y="1597506"/>
+          <a:ext cx="1333076" cy="433865"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Geringer Merhwert,</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>hoher</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1200" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> Aufwand</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1200" kern="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}" name="tblMap" displayName="tblMap" ref="A1:B4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}" name="tblMap" displayName="tblMap" ref="A1:B4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:B4" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2E415323-F0F4-DF42-8618-DFC330E24A9F}" name="Label" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{2AD24CC9-CE9F-3C47-8031-91B2311661C6}" name="Zahl" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{2E415323-F0F4-DF42-8618-DFC330E24A9F}" name="Label" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{2AD24CC9-CE9F-3C47-8031-91B2311661C6}" name="Zahl" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D91CD661-3334-0F41-A7F6-D541C684E11A}" name="tblRaster" displayName="tblRaster" ref="A1:F10" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D91CD661-3334-0F41-A7F6-D541C684E11A}" name="tblRaster" displayName="tblRaster" ref="A1:F10" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:F10" xr:uid="{D91CD661-3334-0F41-A7F6-D541C684E11A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{48EC3C85-0478-E24F-8C6C-9E9150301F82}" name="Zusatzdimension" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2B1F30E9-8D65-194C-8994-DEC140EDE5E1}" name="Unterdimension" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B5FF6543-2649-CE49-AD49-22965AEE247E}" name="Achse" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{48EC3C85-0478-E24F-8C6C-9E9150301F82}" name="Zusatzdimension" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2B1F30E9-8D65-194C-8994-DEC140EDE5E1}" name="Unterdimension" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B5FF6543-2649-CE49-AD49-22965AEE247E}" name="Achse" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{DDD13B20-7639-A54A-84A9-A92CB62DB822}" name="Leitfrage"/>
     <tableColumn id="5" xr3:uid="{A5671AFB-0AFF-BA43-85A5-F8CAA3830C0A}" name="Bewertung"/>
-    <tableColumn id="6" xr3:uid="{9E073365-4767-7540-B07B-6DC0088374EA}" name="Wert" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{9E073365-4767-7540-B07B-6DC0088374EA}" name="Wert" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{08E20751-39CE-A24D-B23A-DFB712B9FFEB}" name="tblMap3" displayName="tblMap3" ref="A1:B4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:B4" xr:uid="{127B5390-E1B3-0C4E-8610-7F4AE37F3B5C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D0189C37-2A96-0344-BD58-635533580973}" name="Label" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{385F4723-0A38-9344-B1F9-694C77879BC9}" name="Zahl" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2B325C1F-ACEB-0042-BFE6-EAEF743DAF32}" name="tblRaster5" displayName="tblRaster5" ref="A1:H10" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:H10" xr:uid="{D91CD661-3334-0F41-A7F6-D541C684E11A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{5C4BC78A-6999-9F4A-804F-1758DFD47407}" name="Zusatzdimension" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{99B900AF-8530-9B47-8A2C-F0B438D3D16A}" name="Unterdimension" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{58444EF8-9A2D-5548-898F-B82492CD709B}" name="Achse" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{24972EC0-7015-A345-88E9-5BCC7AFF8540}" name="Leitfrage"/>
+    <tableColumn id="5" xr3:uid="{0767AE67-88C7-E140-91E3-F0D319268469}" name="Bewertung"/>
+    <tableColumn id="6" xr3:uid="{2AED5FBF-571F-B841-B595-17310A18A286}" name="Wert" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{F3C7ACF5-96BE-6E48-8FD3-A8F08A2EB16E}" name="Gewicht"/>
+    <tableColumn id="8" xr3:uid="{802A9BEB-D4AE-0C41-914F-8E3E42FF0DA7}" name="GewichteterWert" dataDxfId="0">
+      <calculatedColumnFormula>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2562,7 +4469,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="168" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2608,11 +4515,11 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2671,11 +4578,11 @@
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2692,11 +4599,11 @@
         <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2755,11 +4662,11 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -2776,11 +4683,11 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <f>_xlfn.XLOOKUP(tblRaster[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2823,8 +4730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C8DB19-1CE3-7244-8251-0376F2D8C384}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2854,7 +4761,7 @@
     (tblRaster[Achse]="X")+(tblRaster[Achse]="X+Y")
   )
 )</f>
-        <v>1.8571428571428572</v>
+        <v>1.5714285714285714</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2918,7 +4825,7 @@
       </c>
       <c r="B12">
         <f>B3</f>
-        <v>1.8571428571428572</v>
+        <v>1.5714285714285714</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2975,7 +4882,567 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53922EB4-A90D-3D42-9580-538B95E9FA6F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="110" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A66D83-F865-2740-9EA5-CB56A01A2BB9}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="59.6640625" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.XLOOKUP(tblRaster5[[#This Row],[Bewertung]],tblMap[Label],tblMap[Zahl])</f>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f>tblRaster5[[#This Row],[Wert]]*tblRaster5[[#This Row],[Gewicht]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C11:C60" xr:uid="{AC4204A0-0C45-684B-8DDD-2400AB29C86C}">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"X, Y, X+Y"</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"X, Y, X+Y"</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Wert eingeben" sqref="E11:E56" xr:uid="{785B6643-4C70-C840-A919-53A6D8A1FF0A}">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"niedrig,mittel,hoch "</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"niedrig,mittel,hoch "</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25975464-FE90-5E43-862D-639EE3B673F9}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" cm="1">
+        <f t="array" ref="B3">SUM(
+  _xlfn._xlws.FILTER(tblRaster5[GewichteterWert],
+    (tblRaster5[Achse]="X")+(tblRaster5[Achse]="X+Y")
+  )
+)
+/SUM(
+  _xlfn._xlws.FILTER(tblRaster5[Gewicht],
+    (tblRaster5[Achse]="X")+(tblRaster5[Achse]="X+Y")
+  )
+)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" cm="1">
+        <f t="array" ref="B4">SUM(
+  _xlfn._xlws.FILTER(tblRaster5[GewichteterWert],
+    (tblRaster5[Achse]="Y")+(tblRaster5[Achse]="X+Y")
+  )
+)
+/SUM(
+  _xlfn._xlws.FILTER(tblRaster5[Gewicht],
+    (tblRaster5[Achse]="Y")+(tblRaster5[Achse]="X+Y")
+  )
+)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <f>IF(B3&gt;=$B$1,"hoch","niedrig")</f>
+        <v>niedrig</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f>IF(B4&gt;=$B$1,"hoch","niedrig")</f>
+        <v>hoch</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <f>B7&amp;"/"&amp;B6</f>
+        <v>hoch/niedrig</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="str">
+        <f>IF(COUNTBLANK(tblRaster[Bewertung])=0,"ok","fehlt")</f>
+        <v>ok</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <f>B3</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <f>B4</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
fix: 05_03 Checkliste Optik verbessert
</commit_message>
<xml_diff>
--- a/Excel/05_03_checkliste.xlsx
+++ b/Excel/05_03_checkliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D2C707-AFB8-544E-82B1-148027F876A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0585D2A6-FA1C-C348-AB5F-DB89CDFFAD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{824E35B1-06FB-A441-A126-FF76D37EF72C}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{824E35B1-06FB-A441-A126-FF76D37EF72C}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -1266,7 +1266,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9489993D-EBE9-074B-AE6A-4197D1C95890}" type="CELLRANGE">
+                    <a:fld id="{309A475E-89A5-3B41-B53D-78D3F3496695}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -3460,16 +3460,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>742752</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>21392</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>162316</xdr:rowOff>
+      <xdr:rowOff>50556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>91439</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4952,7 +4952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A66D83-F865-2740-9EA5-CB56A01A2BB9}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -5280,8 +5280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25975464-FE90-5E43-862D-639EE3B673F9}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>